<commit_message>
1.08 + deprecate previous versions
</commit_message>
<xml_diff>
--- a/AFR-Tables/Versatune-AFR-231HP.xlsx
+++ b/AFR-Tables/Versatune-AFR-231HP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LOW\RX8-E85-Vtune\AFR-Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E894A387-071B-408F-A73D-994B60DFDAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B0268B-9E44-4D99-A0DF-7AA2CA82DC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{2514486D-E812-4022-A966-38CF6771A7CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2514486D-E812-4022-A966-38CF6771A7CB}"/>
   </bookViews>
   <sheets>
     <sheet name="AFR1 Versatune Stock" sheetId="1" r:id="rId1"/>
@@ -386,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA4637B-1BCC-4C54-9DC4-4D6D8FC3955E}">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,6 +1627,1640 @@
       </c>
       <c r="U19" s="1">
         <v>10.16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>A1/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ref="B22:U22" si="0">B1/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" ref="A23:U23" si="1">A2/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" ref="A24:U24" si="2">A3/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="2"/>
+        <v>0.94557823129251706</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="2"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="2"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="2"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="2"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="2"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="2"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="2"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="2"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="2"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="2"/>
+        <v>0.94149659863945578</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" ref="A25:U25" si="3">A4/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="3"/>
+        <v>0.96462585034013604</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>0.96462585034013604</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="3"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="3"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="3"/>
+        <v>0.85918367346938784</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="3"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="3"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="3"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="3"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="3"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="3"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="3"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="3"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="3"/>
+        <v>0.87142857142857155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" ref="A26:U26" si="4">A5/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="4"/>
+        <v>0.96462585034013604</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="4"/>
+        <v>0.96462585034013604</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="4"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="4"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="4"/>
+        <v>0.85170068027210888</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="4"/>
+        <v>0.85918367346938784</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="4"/>
+        <v>0.85918367346938784</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="4"/>
+        <v>0.85918367346938784</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="4"/>
+        <v>0.85918367346938784</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="4"/>
+        <v>0.85918367346938784</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="4"/>
+        <v>0.85918367346938784</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="4"/>
+        <v>0.85918367346938784</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="4"/>
+        <v>0.85918367346938784</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="4"/>
+        <v>0.85918367346938784</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" ref="A27:U27" si="5">A6/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="5"/>
+        <v>0.96462585034013604</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="5"/>
+        <v>0.96462585034013604</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="5"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="5"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="5"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="5"/>
+        <v>0.85170068027210888</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="5"/>
+        <v>0.85918367346938784</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="5"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="5"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="5"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="5"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="5"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="5"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="5"/>
+        <v>0.87142857142857155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" ref="A28:U28" si="6">A7/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="6"/>
+        <v>0.96462585034013604</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="6"/>
+        <v>0.96462585034013604</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="6"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="6"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="6"/>
+        <v>0.87891156462585041</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="6"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="6"/>
+        <v>0.85918367346938784</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="6"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="6"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="6"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="6"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="6"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="6"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="6"/>
+        <v>0.84013605442176875</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" ref="A29:U29" si="7">A8/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="7"/>
+        <v>0.99251700680272115</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="7"/>
+        <v>0.99251700680272115</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="7"/>
+        <v>0.87891156462585041</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="7"/>
+        <v>0.87891156462585041</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="7"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="7"/>
+        <v>0.85918367346938784</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="7"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="7"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="7"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="7"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="7"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="7"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="7"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="7"/>
+        <v>0.78095238095238106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" ref="A30:U30" si="8">A9/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="8"/>
+        <v>0.97278911564625858</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="8"/>
+        <v>0.97278911564625858</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="8"/>
+        <v>0.96870748299319731</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="8"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="8"/>
+        <v>0.85918367346938784</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="8"/>
+        <v>0.85170068027210888</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="8"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="8"/>
+        <v>0.73061224489795928</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="8"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="8"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="8"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="8"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="8"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="8"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="8"/>
+        <v>0.71904761904761905</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" ref="A31:U31" si="9">A10/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="9"/>
+        <v>0.97687074829931975</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="9"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="9"/>
+        <v>0.94557823129251706</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="9"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="9"/>
+        <v>0.85918367346938784</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="9"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="9"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="9"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="9"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="9"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="9"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="9"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="9"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="9"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="9"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="9"/>
+        <v>0.76190476190476186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" ref="A32:U32" si="10">A11/14.7</f>
+        <v>0.92993197278911566</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="10"/>
+        <v>0.92993197278911566</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="10"/>
+        <v>0.92993197278911566</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="10"/>
+        <v>0.91020408163265321</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="10"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="10"/>
+        <v>0.92585034013605438</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="10"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="10"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="10"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="10"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="10"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="10"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="10"/>
+        <v>0.82040816326530619</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="10"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="10"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="10"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="10"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="10"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="10"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="10"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="10"/>
+        <v>0.76190476190476186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" ref="A33:U33" si="11">A12/14.7</f>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="11"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="11"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="11"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="11"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="11"/>
+        <v>0.91428571428571426</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="11"/>
+        <v>0.88299319727891168</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="11"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="11"/>
+        <v>0.85170068027210888</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="11"/>
+        <v>0.89863945578231308</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="11"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="11"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="11"/>
+        <v>0.86734693877551028</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="11"/>
+        <v>0.83197278911564632</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="11"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="11"/>
+        <v>0.78503401360544212</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="11"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="11"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="11"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="11"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="11"/>
+        <v>0.79659863945578246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" ref="A34:U34" si="12">A13/14.7</f>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="12"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="12"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="12"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="12"/>
+        <v>0.88299319727891168</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="12"/>
+        <v>0.89863945578231308</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="12"/>
+        <v>0.88299319727891168</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="12"/>
+        <v>0.87891156462585041</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="12"/>
+        <v>0.86734693877551028</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="12"/>
+        <v>0.86326530612244901</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="12"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="12"/>
+        <v>0.87891156462585041</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="12"/>
+        <v>0.82040816326530619</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="12"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="12"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="12"/>
+        <v>0.76530612244897966</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="12"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="12"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="12"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="12"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="12"/>
+        <v>0.75374149659863954</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" ref="A35:U35" si="13">A14/14.7</f>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="13"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="13"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="13"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="13"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="13"/>
+        <v>0.85170068027210888</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="13"/>
+        <v>0.89047619047619053</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="13"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="13"/>
+        <v>0.85170068027210888</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="13"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="13"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="13"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="13"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="13"/>
+        <v>0.77755102040816326</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="13"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="13"/>
+        <v>0.72653061224489801</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="13"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="13"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="13"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="13"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="13"/>
+        <v>0.71904761904761905</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" ref="A36:U36" si="14">A15/14.7</f>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="14"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="14"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="14"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="14"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="14"/>
+        <v>0.81224489795918364</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="14"/>
+        <v>0.83197278911564632</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="14"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="14"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="14"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="14"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="14"/>
+        <v>0.77755102040816326</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="14"/>
+        <v>0.75034013605442174</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="14"/>
+        <v>0.71088435374149661</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="14"/>
+        <v>0.71088435374149661</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="14"/>
+        <v>0.6796598639455782</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="14"/>
+        <v>0.6796598639455782</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="14"/>
+        <v>0.6796598639455782</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="14"/>
+        <v>0.6796598639455782</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="14"/>
+        <v>0.6796598639455782</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="14"/>
+        <v>0.6796598639455782</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" ref="A37:U37" si="15">A16/14.7</f>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="15"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="15"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="15"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="15"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="15"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="15"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="15"/>
+        <v>0.82040816326530619</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="15"/>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="15"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="15"/>
+        <v>0.76938775510204094</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="15"/>
+        <v>0.73469387755102045</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="15"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="15"/>
+        <v>0.73061224489795928</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="15"/>
+        <v>0.71496598639455788</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="15"/>
+        <v>0.70680272108843545</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="15"/>
+        <v>0.70680272108843545</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="15"/>
+        <v>0.70680272108843545</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="15"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="15"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="15"/>
+        <v>0.71904761904761905</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" ref="A38:U38" si="16">A17/14.7</f>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="16"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="16"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="16"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="16"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="16"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="16"/>
+        <v>0.77755102040816326</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="16"/>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="16"/>
+        <v>0.82789115646258504</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="16"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="16"/>
+        <v>0.76530612244897966</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="16"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="16"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="16"/>
+        <v>0.73469387755102045</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="16"/>
+        <v>0.73061224489795928</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="16"/>
+        <v>0.69931972789115648</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="16"/>
+        <v>0.69115646258503405</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="16"/>
+        <v>0.69523809523809532</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="16"/>
+        <v>0.72653061224489801</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="16"/>
+        <v>0.72653061224489801</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="16"/>
+        <v>0.72653061224489801</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" ref="A39:U39" si="17">A18/14.7</f>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="17"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="17"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="17"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="17"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="17"/>
+        <v>0.76938775510204094</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="17"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="17"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="17"/>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="17"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="17"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="17"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="17"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="17"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="17"/>
+        <v>0.71496598639455788</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="17"/>
+        <v>0.69115646258503405</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="17"/>
+        <v>0.69115646258503405</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="17"/>
+        <v>0.69115646258503405</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="17"/>
+        <v>0.69115646258503405</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="17"/>
+        <v>0.69115646258503405</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="17"/>
+        <v>0.69115646258503405</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" ref="A40:U40" si="18">A19/14.7</f>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="18"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="18"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="18"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="18"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="18"/>
+        <v>0.76938775510204094</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="18"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="18"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="18"/>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="18"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="18"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="18"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="18"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="18"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="18"/>
+        <v>0.71496598639455788</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="18"/>
+        <v>0.69115646258503405</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="18"/>
+        <v>0.69115646258503405</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="18"/>
+        <v>0.69115646258503405</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="18"/>
+        <v>0.69115646258503405</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="18"/>
+        <v>0.69115646258503405</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="18"/>
+        <v>0.69115646258503405</v>
       </c>
     </row>
   </sheetData>
@@ -1636,10 +3270,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358C10B9-2BEF-4F95-9FE1-0F2E25206362}">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:U19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:U40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,6 +4511,1640 @@
       </c>
       <c r="U19" s="1">
         <v>11.08</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>A1/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ref="B22:U22" si="0">B1/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" ref="A23:U35" si="1">A2/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>0.94557823129251706</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="1"/>
+        <v>0.93333333333333346</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>0.92993197278911566</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="1"/>
+        <v>0.92993197278911566</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>0.99591836734693884</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="1"/>
+        <v>0.99591836734693884</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>0.96122448979591846</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>0.99251700680272115</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>0.99251700680272115</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>0.96462585034013604</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="1"/>
+        <v>0.96122448979591846</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="1"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="1"/>
+        <v>0.86326530612244901</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>0.97278911564625858</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>0.97278911564625858</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>0.96870748299319731</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="1"/>
+        <v>0.92585034013605438</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="1"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="1"/>
+        <v>0.81224489795918364</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="1"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="1"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="1"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="1"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="1"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="1"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="1"/>
+        <v>0.80068027210884352</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>0.97687074829931975</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>0.94557823129251706</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="1"/>
+        <v>0.89047619047619053</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>0.86734693877551028</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="1"/>
+        <v>0.88299319727891168</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>0.87482993197278913</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="1"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="1"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="1"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="1"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="1"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="1"/>
+        <v>0.84013605442176875</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="1"/>
+        <v>0.92993197278911566</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="1"/>
+        <v>0.92993197278911566</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>0.92993197278911566</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>0.91020408163265321</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0.92585034013605438</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>0.89047619047619053</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="1"/>
+        <v>0.87891156462585041</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="1"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="1"/>
+        <v>0.90204081632653066</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="1"/>
+        <v>0.87482993197278913</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="1"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="1"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="1"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="1"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="1"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="1"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="1"/>
+        <v>0.83605442176870748</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="1"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="1"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0.91428571428571426</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>0.88299319727891168</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>0.85170068027210888</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>0.89863945578231308</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="1"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="1"/>
+        <v>0.86734693877551028</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="1"/>
+        <v>0.83197278911564632</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="1"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="1"/>
+        <v>0.78503401360544212</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="1"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="1"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>0.88299319727891168</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0.89863945578231308</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>0.88299319727891168</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>0.87891156462585041</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>0.86734693877551028</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="1"/>
+        <v>0.86326530612244901</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="1"/>
+        <v>0.87891156462585041</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="1"/>
+        <v>0.82040816326530619</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="1"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="1"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="1"/>
+        <v>0.78503401360544212</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="1"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ref="D35:U35" si="2">D14/14.7</f>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>0.85170068027210888</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="2"/>
+        <v>0.89047619047619053</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="2"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="2"/>
+        <v>0.85170068027210888</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="2"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="2"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="2"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="2"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="2"/>
+        <v>0.77755102040816326</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="2"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="2"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="2"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="2"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="2"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="2"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="2"/>
+        <v>0.80476190476190479</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" ref="A36:U40" si="3">A15/14.7</f>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="3"/>
+        <v>0.81224489795918364</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="3"/>
+        <v>0.83197278911564632</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="3"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="3"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="3"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="3"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="3"/>
+        <v>0.77755102040816326</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="3"/>
+        <v>0.75034013605442174</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="3"/>
+        <v>0.71088435374149661</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="3"/>
+        <v>0.71088435374149661</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="3"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="3"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="3"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="3"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="3"/>
+        <v>0.80884353741496606</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="3"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="3"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="3"/>
+        <v>0.82040816326530619</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="3"/>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="3"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="3"/>
+        <v>0.76938775510204094</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="3"/>
+        <v>0.73469387755102045</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="3"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="3"/>
+        <v>0.73061224489795928</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="3"/>
+        <v>0.71496598639455788</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="3"/>
+        <v>0.82040816326530619</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="3"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="3"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="3"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="3"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="3"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="3"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="3"/>
+        <v>0.77755102040816326</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="3"/>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="3"/>
+        <v>0.82789115646258504</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="3"/>
+        <v>0.76530612244897966</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="3"/>
+        <v>0.73469387755102045</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="3"/>
+        <v>0.73061224489795928</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="3"/>
+        <v>0.76530612244897966</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="3"/>
+        <v>0.76530612244897966</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="3"/>
+        <v>0.76530612244897966</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="3"/>
+        <v>0.76530612244897966</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="3"/>
+        <v>0.76530612244897966</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="3"/>
+        <v>0.76530612244897966</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="3"/>
+        <v>0.76938775510204094</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="3"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="3"/>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="3"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="3"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="3"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="3"/>
+        <v>0.76938775510204094</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="3"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="3"/>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="3"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="3"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="3"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
       </c>
     </row>
   </sheetData>
@@ -2886,10 +6154,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6632C126-0F68-4DBE-A89D-4A17345EBF12}">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4127,6 +7395,1640 @@
       </c>
       <c r="U19" s="1">
         <v>11.08</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>A1/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ref="B22:U22" si="0">B1/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" ref="A23:U35" si="1">A2/14.7</f>
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="1"/>
+        <v>0.95714285714285718</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>0.94557823129251706</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="1"/>
+        <v>0.93333333333333346</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>0.92993197278911566</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="1"/>
+        <v>0.92993197278911566</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>0.94149659863945578</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>0.99591836734693884</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="1"/>
+        <v>0.99591836734693884</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>0.96122448979591846</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>0.99251700680272115</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>0.99251700680272115</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>0.96462585034013604</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="1"/>
+        <v>0.96122448979591846</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="1"/>
+        <v>0.93741496598639451</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="1"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="1"/>
+        <v>0.86326530612244901</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>0.99591836734693884</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>0.99591836734693884</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>0.98027210884353744</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="1"/>
+        <v>0.98843537414965987</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="1"/>
+        <v>0.99251700680272115</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="1"/>
+        <v>0.96870748299319731</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="1"/>
+        <v>0.89047619047619053</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="1"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="1"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="1"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="1"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="1"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="1"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="1"/>
+        <v>0.80068027210884352</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>0.99591836734693884</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>0.99591836734693884</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>0.99591836734693884</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>0.98843537414965987</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>0.96870748299319731</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="1"/>
+        <v>0.93333333333333346</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>0.89047619047619053</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="1"/>
+        <v>0.89047619047619053</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>0.94897959183673464</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="1"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="1"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="1"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="1"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="1"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="1"/>
+        <v>0.84013605442176875</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>0.98843537414965987</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>0.96462585034013604</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0.96870748299319731</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>0.99591836734693884</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>0.97687074829931975</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>0.94557823129251706</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>0.89047619047619053</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="1"/>
+        <v>0.89047619047619053</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="1"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="1"/>
+        <v>0.96462585034013604</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="1"/>
+        <v>0.94557823129251706</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="1"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="1"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="1"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="1"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="1"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="1"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="1"/>
+        <v>0.83605442176870748</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>0.87482993197278913</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0.92176870748299333</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>0.91428571428571426</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>0.89455782312925181</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>0.86734693877551028</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>0.86326530612244901</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="1"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>0.88639455782312926</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="1"/>
+        <v>0.91428571428571426</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="1"/>
+        <v>0.95306122448979591</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="1"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="1"/>
+        <v>0.78503401360544212</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="1"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="1"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>0.88299319727891168</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0.89863945578231308</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>0.88299319727891168</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>0.87891156462585041</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>0.86734693877551028</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="1"/>
+        <v>0.86326530612244901</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="1"/>
+        <v>0.85578231292517015</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="1"/>
+        <v>0.87891156462585041</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="1"/>
+        <v>0.82040816326530619</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="1"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="1"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="1"/>
+        <v>0.78503401360544212</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="1"/>
+        <v>0.79659863945578246</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="1"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ref="D35:U35" si="2">D14/14.7</f>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>0.85170068027210888</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="2"/>
+        <v>0.89047619047619053</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="2"/>
+        <v>0.87142857142857155</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="2"/>
+        <v>0.85170068027210888</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="2"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="2"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="2"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="2"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="2"/>
+        <v>0.77755102040816326</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="2"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="2"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="2"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="2"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="2"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="2"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="2"/>
+        <v>0.80476190476190479</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" ref="A36:U40" si="3">A15/14.7</f>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="3"/>
+        <v>0.81224489795918364</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="3"/>
+        <v>0.83197278911564632</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="3"/>
+        <v>0.83605442176870748</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="3"/>
+        <v>0.84013605442176875</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="3"/>
+        <v>0.82448979591836735</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="3"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="3"/>
+        <v>0.77755102040816326</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="3"/>
+        <v>0.75034013605442174</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="3"/>
+        <v>0.71088435374149661</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="3"/>
+        <v>0.71088435374149661</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="3"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="3"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="3"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="3"/>
+        <v>0.80884353741496606</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="3"/>
+        <v>0.80884353741496606</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="3"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="3"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="3"/>
+        <v>0.82040816326530619</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="3"/>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="3"/>
+        <v>0.80068027210884352</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="3"/>
+        <v>0.76938775510204094</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="3"/>
+        <v>0.73469387755102045</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="3"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="3"/>
+        <v>0.73061224489795928</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="3"/>
+        <v>0.71496598639455788</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="3"/>
+        <v>0.82040816326530619</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="3"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="3"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="3"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="3"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="3"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="3"/>
+        <v>0.73809523809523814</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="3"/>
+        <v>0.77755102040816326</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="3"/>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="3"/>
+        <v>0.82789115646258504</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="3"/>
+        <v>0.80476190476190479</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="3"/>
+        <v>0.76530612244897966</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="3"/>
+        <v>0.73469387755102045</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="3"/>
+        <v>0.73061224489795928</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="3"/>
+        <v>0.76530612244897966</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="3"/>
+        <v>0.76530612244897966</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="3"/>
+        <v>0.76530612244897966</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="3"/>
+        <v>0.76530612244897966</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="3"/>
+        <v>0.76530612244897966</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="3"/>
+        <v>0.76530612244897966</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="3"/>
+        <v>0.76938775510204094</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="3"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="3"/>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="3"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="3"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="3"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="3"/>
+        <v>0.76938775510204094</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238106</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="3"/>
+        <v>0.78911564625850339</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="3"/>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="3"/>
+        <v>0.79319727891156466</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="3"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="3"/>
+        <v>0.74625850340136057</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="3"/>
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="3"/>
+        <v>0.75374149659863954</v>
       </c>
     </row>
   </sheetData>
@@ -4138,7 +9040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F35C75B1-49F6-46ED-8DB8-0348CB31F616}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>

</xml_diff>